<commit_message>
Agregar Bloqueo de Ordenes de Compra y de Pedidos, mientras la solicitud de Cancelacion o Cierre se encuentre en estado Pendiente.
uitar de Shipping e Inprocesos los pedidos que tengan soliitud de cancelaion o cierre pendiente de Aprobacion, para que nbo puedan ser prcesados mientras no se de respuesta a la solicitud

Agregar al menu de la aplicacion las 2 nuevas opciones de Gestion de solicitudes Operativas
</commit_message>
<xml_diff>
--- a/documentos/Contrato y Cuentas de Cobro/Control de Cambios Noviembre 2024/2024-11-17 Propuesta Noviembre Aldebaran.xlsx
+++ b/documentos/Contrato y Cuentas de Cobro/Control de Cambios Noviembre 2024/2024-11-17 Propuesta Noviembre Aldebaran.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Promos\Repos\AldebaranWeb\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Promos\Repos\AldebaranWeb\documentos\Contrato y Cuentas de Cobro\Control de Cambios Noviembre 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1830" windowWidth="28800" windowHeight="12105"/>
+    <workbookView xWindow="0" yWindow="2745" windowWidth="28800" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -230,6 +236,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +531,7 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>33</v>
       </c>
@@ -530,33 +539,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -564,7 +576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -572,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -580,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -588,7 +600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -596,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -604,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -612,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
@@ -620,282 +632,294 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
       <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>12</v>
+      <c r="B51" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59">
-        <f>SUM(C4:C57)</f>
-        <v>145</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60">
+        <f>SUM(C4:C58)</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="6">
-        <f>C59/8</f>
+      <c r="C61" s="6">
+        <f>C60/8</f>
         <v>18.125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalizacion Implementacion de Solicitud OIperativa para cancelacion de OC y Pedidos y CIerre de Pedidos.
Independizar los permisos de la solicitud de Cancelacion de la de cierre tanto para OC como para Pedidos

Cambiio de version para despliegue a p´roduccion
</commit_message>
<xml_diff>
--- a/documentos/Contrato y Cuentas de Cobro/Control de Cambios Noviembre 2024/2024-11-17 Propuesta Noviembre Aldebaran.xlsx
+++ b/documentos/Contrato y Cuentas de Cobro/Control de Cambios Noviembre 2024/2024-11-17 Propuesta Noviembre Aldebaran.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2745" windowWidth="28800" windowHeight="12105"/>
+    <workbookView xWindow="0" yWindow="3660" windowWidth="28800" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>- Consultas de Log de Cancelaciones y de Modificaciones para Pedidos, Reservas y Ordenes de Compra</t>
   </si>
@@ -47,9 +47,6 @@
     <t>- Pagina de configuracion de aprobadores para cancelacion de OC y Pedido</t>
   </si>
   <si>
-    <t>Modificar reporte de Pedidos ara mostrar el aprobador cuando el pedido se encuentre cancelado</t>
-  </si>
-  <si>
     <t>Modificar reporte de ordenes de compra para mostrar el aprobador cuando al orden de compra se encuentre cancelada</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>Duracion Velocity de 8 Horas</t>
+  </si>
+  <si>
+    <t>Modificar opcion de cierre de pedidos para crear el registro de solicitud de aprobacion para el cierre dejando pendiente el cambio de estado para cuando la solicitud sea aprobada</t>
+  </si>
+  <si>
+    <t>Modificar reporte de pedidos para mostrar el aprobador cuando el pedido se encuentre cancelado</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +536,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,12 +567,12 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
@@ -577,7 +580,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C8">
@@ -585,8 +588,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -594,7 +597,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -602,63 +605,63 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>10</v>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>9</v>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -666,26 +669,26 @@
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,36 +696,36 @@
         <v>25</v>
       </c>
       <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>3</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -730,34 +733,34 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34">
         <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -765,36 +768,36 @@
         <v>25</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>4</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="B39" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -802,47 +805,47 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>5</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -855,16 +858,16 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C52">
-        <v>6</v>
-      </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
@@ -876,50 +879,58 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C56">
-        <v>6</v>
-      </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C57">
         <v>6</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C59">
         <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60">
-        <f>SUM(C4:C58)</f>
-        <v>145</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="6">
-        <f>C60/8</f>
+        <v>39</v>
+      </c>
+      <c r="C61">
+        <f>SUM(C4:C59)</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="6">
+        <f>C61/8</f>
         <v>18.125</v>
       </c>
     </row>

</xml_diff>